<commit_message>
update data processing and new data script, update images
</commit_message>
<xml_diff>
--- a/data_processing/Weihnachtsmarkt_Bilder.xlsx
+++ b/data_processing/Weihnachtsmarkt_Bilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiakeuss/Documents/GitHub/weihnachtsmarktkarte/data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8FB4BED4-8F87-DA4C-A77D-FF1623EBC682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9736F70C-F16A-6B4E-9DD1-FB942F6CB0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2200" windowWidth="28240" windowHeight="16180" xr2:uid="{6BBC2131-393E-D542-8110-9341F5E7FF08}"/>
+    <workbookView xWindow="2540" yWindow="720" windowWidth="28240" windowHeight="16180" xr2:uid="{6BBC2131-393E-D542-8110-9341F5E7FF08}"/>
   </bookViews>
   <sheets>
     <sheet name="Weihnachtsmarkt_Bilder" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="80">
   <si>
     <t>id</t>
   </si>
@@ -267,6 +267,27 @@
   </si>
   <si>
     <t>Reederei Riedel, CC  Attribution 4.0</t>
+  </si>
+  <si>
+    <t>Christmas_market_Rotes_Rathaus_Berlin.jpg</t>
+  </si>
+  <si>
+    <t>Leonhard Lenz, CC Zero, Public Domain Dedication</t>
+  </si>
+  <si>
+    <t>Eingang_HallenAmBorsigturm.jpg</t>
+  </si>
+  <si>
+    <t>Aiken Hartenfels, CC Attribution-Share Alike 3.0 de</t>
+  </si>
+  <si>
+    <t>weihnachtsmarkt_Breitscheidplatz.jpg</t>
+  </si>
+  <si>
+    <t>Ralf Roletschek, GFDL 1.2 via Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>Christmas_market_Sophienstraße_Berlin.jpg</t>
   </si>
 </sst>
 </file>
@@ -302,9 +323,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -680,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64F4F9-0E9D-A944-A03E-719F3981D4D8}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,13 +730,13 @@
       <c r="A2">
         <v>183</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -724,13 +744,13 @@
       <c r="A3">
         <v>60</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -738,13 +758,13 @@
       <c r="A4">
         <v>63</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -752,13 +772,13 @@
       <c r="A5">
         <v>66</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -766,13 +786,13 @@
       <c r="A6">
         <v>102</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -780,13 +800,13 @@
       <c r="A7">
         <v>105</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -794,13 +814,13 @@
       <c r="A8">
         <v>108</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -808,13 +828,13 @@
       <c r="A9">
         <v>111</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -822,13 +842,13 @@
       <c r="A10">
         <v>99</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -836,13 +856,13 @@
       <c r="A11">
         <v>84</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -850,13 +870,13 @@
       <c r="A12">
         <v>147</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -864,13 +884,13 @@
       <c r="A13">
         <v>93</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -878,13 +898,13 @@
       <c r="A14">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -892,13 +912,13 @@
       <c r="A15">
         <v>144</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -906,13 +926,13 @@
       <c r="A16">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -920,13 +940,13 @@
       <c r="A17">
         <v>114</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -934,13 +954,13 @@
       <c r="A18">
         <v>117</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -948,13 +968,13 @@
       <c r="A19">
         <v>75</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -962,13 +982,13 @@
       <c r="A20">
         <v>78</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -976,13 +996,13 @@
       <c r="A21">
         <v>81</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -990,13 +1010,13 @@
       <c r="A22">
         <v>72</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1004,13 +1024,13 @@
       <c r="A23">
         <v>189</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1018,13 +1038,13 @@
       <c r="A24">
         <v>90</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1032,13 +1052,13 @@
       <c r="A25">
         <v>129</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1046,13 +1066,13 @@
       <c r="A26">
         <v>168</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1060,13 +1080,13 @@
       <c r="A27">
         <v>171</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1074,13 +1094,13 @@
       <c r="A28">
         <v>150</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1088,13 +1108,13 @@
       <c r="A29">
         <v>177</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1102,13 +1122,13 @@
       <c r="A30">
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1116,13 +1136,13 @@
       <c r="A31">
         <v>6</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1130,13 +1150,13 @@
       <c r="A32">
         <v>48</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1144,13 +1164,13 @@
       <c r="A33">
         <v>24</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1158,13 +1178,13 @@
       <c r="A34">
         <v>156</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1172,13 +1192,13 @@
       <c r="A35">
         <v>54</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1186,13 +1206,13 @@
       <c r="A36">
         <v>87</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1200,13 +1220,13 @@
       <c r="A37">
         <v>39</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1214,13 +1234,13 @@
       <c r="A38">
         <v>165</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1228,13 +1248,13 @@
       <c r="A39">
         <v>180</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1242,13 +1262,13 @@
       <c r="A40">
         <v>138</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1256,13 +1276,13 @@
       <c r="A41">
         <v>162</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1270,13 +1290,13 @@
       <c r="A42">
         <v>57</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1284,13 +1304,13 @@
       <c r="A43">
         <v>27</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1298,13 +1318,13 @@
       <c r="A44">
         <v>51</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1312,27 +1332,27 @@
       <c r="A45">
         <v>3</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>5</v>
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>186</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1340,13 +1360,13 @@
       <c r="A47">
         <v>12</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>45</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1354,27 +1374,27 @@
       <c r="A48">
         <v>15</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>5</v>
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>42</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1382,13 +1402,13 @@
       <c r="A50">
         <v>141</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1396,13 +1416,13 @@
       <c r="A51">
         <v>135</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1410,13 +1430,13 @@
       <c r="A52">
         <v>132</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1424,13 +1444,13 @@
       <c r="A53">
         <v>69</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1438,13 +1458,13 @@
       <c r="A54">
         <v>123</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1452,27 +1472,27 @@
       <c r="A55">
         <v>174</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>5</v>
+      <c r="C55" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>96</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1480,13 +1500,13 @@
       <c r="A57">
         <v>126</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="1" t="s">
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1494,13 +1514,13 @@
       <c r="A58">
         <v>45</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="1" t="s">
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1508,13 +1528,13 @@
       <c r="A59">
         <v>18</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>64</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="1" t="s">
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1522,27 +1542,27 @@
       <c r="A60">
         <v>153</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>5</v>
+      <c r="C60" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>159</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1550,13 +1570,13 @@
       <c r="A62">
         <v>120</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1564,13 +1584,13 @@
       <c r="A63">
         <v>33</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1578,13 +1598,13 @@
       <c r="A64">
         <v>9</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>